<commit_message>
disposition form , readme
</commit_message>
<xml_diff>
--- a/Demo Deliveries.xlsx
+++ b/Demo Deliveries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\new synertics\forked\SynerticsDev\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\synerticsOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEF4E6E-DD9B-4465-980E-C8AB099D7DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4890434A-576B-46F8-B69C-B33FACA57509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1200" windowWidth="25335" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,10 +506,10 @@
         <v>29</v>
       </c>
       <c r="C2" s="3">
-        <v>44426.354166666664</v>
+        <v>44791.354166666664</v>
       </c>
       <c r="D2" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -520,10 +520,10 @@
         <v>28</v>
       </c>
       <c r="C3" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D3" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,10 +534,10 @@
         <v>29</v>
       </c>
       <c r="C4" s="3">
-        <v>44426.354166666664</v>
+        <v>44791.354166666664</v>
       </c>
       <c r="D4" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,10 +548,10 @@
         <v>30</v>
       </c>
       <c r="C5" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D5" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,10 +562,10 @@
         <v>31</v>
       </c>
       <c r="C6" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D6" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -576,10 +576,10 @@
         <v>32</v>
       </c>
       <c r="C7" s="3">
-        <v>44426.354166666664</v>
+        <v>44791.354166666664</v>
       </c>
       <c r="D7" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,10 +590,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D8" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,10 +604,10 @@
         <v>34</v>
       </c>
       <c r="C9" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D9" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,10 +618,10 @@
         <v>35</v>
       </c>
       <c r="C10" s="3">
-        <v>44426.354166666664</v>
+        <v>44791.354166666664</v>
       </c>
       <c r="D10" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,10 +632,10 @@
         <v>36</v>
       </c>
       <c r="C11" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D11" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,10 +646,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D12" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,10 +660,10 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>44426.6875</v>
+        <v>44791.6875</v>
       </c>
       <c r="D13" s="2">
-        <v>44426.770833333336</v>
+        <v>44791.770833333336</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,10 +674,10 @@
         <v>29</v>
       </c>
       <c r="C14" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
       <c r="D14" s="3">
-        <v>44426.729166666664</v>
+        <v>44791.729166666664</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,10 +688,10 @@
         <v>30</v>
       </c>
       <c r="C15" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
       <c r="D15" s="3">
-        <v>44426.729166666664</v>
+        <v>44791.729166666664</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,10 +702,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="2">
-        <v>44426.6875</v>
+        <v>44791.6875</v>
       </c>
       <c r="D16" s="2">
-        <v>44426.770833333336</v>
+        <v>44791.770833333336</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,10 +716,10 @@
         <v>32</v>
       </c>
       <c r="C17" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
       <c r="D17" s="3">
-        <v>44426.729166666664</v>
+        <v>44791.729166666664</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,10 +730,10 @@
         <v>33</v>
       </c>
       <c r="C18" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
       <c r="D18" s="3">
-        <v>44426.729166666664</v>
+        <v>44791.729166666664</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,10 +744,10 @@
         <v>34</v>
       </c>
       <c r="C19" s="2">
-        <v>44426.6875</v>
+        <v>44791.6875</v>
       </c>
       <c r="D19" s="2">
-        <v>44426.770833333336</v>
+        <v>44791.770833333336</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -758,10 +758,10 @@
         <v>35</v>
       </c>
       <c r="C20" s="2">
-        <v>44426.6875</v>
+        <v>44791.6875</v>
       </c>
       <c r="D20" s="2">
-        <v>44426.770833333336</v>
+        <v>44791.770833333336</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -772,10 +772,10 @@
         <v>36</v>
       </c>
       <c r="C21" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D21" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,10 +786,10 @@
         <v>27</v>
       </c>
       <c r="C22" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D22" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -800,10 +800,10 @@
         <v>28</v>
       </c>
       <c r="C23" s="3">
-        <v>44426.354166666664</v>
+        <v>44791.354166666664</v>
       </c>
       <c r="D23" s="2">
-        <v>44426.5625</v>
+        <v>44791.5625</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -814,10 +814,10 @@
         <v>29</v>
       </c>
       <c r="C24" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D24" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,10 +828,10 @@
         <v>30</v>
       </c>
       <c r="C25" s="2">
-        <v>44426.395833333336</v>
+        <v>44791.395833333336</v>
       </c>
       <c r="D25" s="3">
-        <v>44426.520833333336</v>
+        <v>44791.520833333336</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>